<commit_message>
Andere Skalierung mit Smallsort
</commit_message>
<xml_diff>
--- a/Ausarbeitung/Test_Diagramme_zumAbgeben.xlsx
+++ b/Ausarbeitung/Test_Diagramme_zumAbgeben.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -566,11 +569,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="346217616"/>
-        <c:axId val="346237608"/>
+        <c:axId val="449529040"/>
+        <c:axId val="449532960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346217616"/>
+        <c:axId val="449529040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +616,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346237608"/>
+        <c:crossAx val="449532960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -621,7 +624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346237608"/>
+        <c:axId val="449532960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,7 +675,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346217616"/>
+        <c:crossAx val="449529040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1085,11 +1088,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347268528"/>
-        <c:axId val="347268920"/>
+        <c:axId val="449538056"/>
+        <c:axId val="449537664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347268528"/>
+        <c:axId val="449538056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1135,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347268920"/>
+        <c:crossAx val="449537664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1140,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347268920"/>
+        <c:axId val="449537664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1194,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347268528"/>
+        <c:crossAx val="449538056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1325,7 +1328,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1604,11 +1606,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347271664"/>
-        <c:axId val="347269312"/>
+        <c:axId val="449537272"/>
+        <c:axId val="449534920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347271664"/>
+        <c:axId val="449537272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,7 +1653,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347269312"/>
+        <c:crossAx val="449534920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1659,7 +1661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347269312"/>
+        <c:axId val="449534920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1710,7 +1712,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347271664"/>
+        <c:crossAx val="449537272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1725,7 +1727,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2124,11 +2125,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347272448"/>
-        <c:axId val="347272056"/>
+        <c:axId val="449536096"/>
+        <c:axId val="449536488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347272448"/>
+        <c:axId val="449536096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2171,7 +2172,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347272056"/>
+        <c:crossAx val="449536488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2179,7 +2180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347272056"/>
+        <c:axId val="449536488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,7 +2231,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347272448"/>
+        <c:crossAx val="449536096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2643,11 +2644,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347639600"/>
-        <c:axId val="347639208"/>
+        <c:axId val="455398128"/>
+        <c:axId val="455396168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347639600"/>
+        <c:axId val="455398128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2691,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347639208"/>
+        <c:crossAx val="455396168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347639208"/>
+        <c:axId val="455396168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +2750,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347639600"/>
+        <c:crossAx val="455398128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3162,11 +3163,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347643128"/>
-        <c:axId val="347639992"/>
+        <c:axId val="455396952"/>
+        <c:axId val="455397344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347643128"/>
+        <c:axId val="455396952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3209,7 +3210,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347639992"/>
+        <c:crossAx val="455397344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3217,7 +3218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347639992"/>
+        <c:axId val="455397344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3268,7 +3269,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347643128"/>
+        <c:crossAx val="455396952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3682,11 +3683,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347637248"/>
-        <c:axId val="347636464"/>
+        <c:axId val="455398520"/>
+        <c:axId val="455399304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347637248"/>
+        <c:axId val="455398520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,7 +3730,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347636464"/>
+        <c:crossAx val="455399304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3737,7 +3738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347636464"/>
+        <c:axId val="455399304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3789,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347637248"/>
+        <c:crossAx val="455398520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4202,11 +4203,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347640384"/>
-        <c:axId val="347636856"/>
+        <c:axId val="455399696"/>
+        <c:axId val="455397736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347640384"/>
+        <c:axId val="455399696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4249,7 +4250,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347636856"/>
+        <c:crossAx val="455397736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4257,7 +4258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347636856"/>
+        <c:axId val="455397736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4308,7 +4309,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347640384"/>
+        <c:crossAx val="455399696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4721,11 +4722,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347641560"/>
-        <c:axId val="347637640"/>
+        <c:axId val="455400088"/>
+        <c:axId val="455400480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347641560"/>
+        <c:axId val="455400088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4768,7 +4769,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347637640"/>
+        <c:crossAx val="455400480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4776,7 +4777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347637640"/>
+        <c:axId val="455400480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4827,7 +4828,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347641560"/>
+        <c:crossAx val="455400088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5240,11 +5241,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347638424"/>
-        <c:axId val="347641168"/>
+        <c:axId val="455400872"/>
+        <c:axId val="455401264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347638424"/>
+        <c:axId val="455400872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5288,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347641168"/>
+        <c:crossAx val="455401264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5295,7 +5296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347641168"/>
+        <c:axId val="455401264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5346,7 +5347,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347638424"/>
+        <c:crossAx val="455400872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5755,11 +5756,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347635680"/>
-        <c:axId val="347636072"/>
+        <c:axId val="455402440"/>
+        <c:axId val="455402832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347635680"/>
+        <c:axId val="455402440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5802,7 +5803,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347636072"/>
+        <c:crossAx val="455402832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5810,7 +5811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347636072"/>
+        <c:axId val="455402832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5861,7 +5862,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347635680"/>
+        <c:crossAx val="455402440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6393,11 +6394,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="345805184"/>
-        <c:axId val="346694896"/>
+        <c:axId val="449522768"/>
+        <c:axId val="449533352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345805184"/>
+        <c:axId val="449522768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6440,7 +6441,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346694896"/>
+        <c:crossAx val="449533352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6448,7 +6449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346694896"/>
+        <c:axId val="449533352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6499,7 +6500,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345805184"/>
+        <c:crossAx val="449522768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6908,11 +6909,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348543328"/>
-        <c:axId val="348542152"/>
+        <c:axId val="455393032"/>
+        <c:axId val="455393424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348543328"/>
+        <c:axId val="455393032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6955,7 +6956,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348542152"/>
+        <c:crossAx val="455393424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6963,7 +6964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348542152"/>
+        <c:axId val="455393424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7014,7 +7015,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348543328"/>
+        <c:crossAx val="455393032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7423,11 +7424,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348544112"/>
-        <c:axId val="348542936"/>
+        <c:axId val="455404792"/>
+        <c:axId val="455392640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348544112"/>
+        <c:axId val="455404792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7470,7 +7471,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348542936"/>
+        <c:crossAx val="455392640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7478,7 +7479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348542936"/>
+        <c:axId val="455392640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7529,7 +7530,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348544112"/>
+        <c:crossAx val="455404792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8070,11 +8071,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348536664"/>
-        <c:axId val="348537840"/>
+        <c:axId val="455405968"/>
+        <c:axId val="455407928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348536664"/>
+        <c:axId val="455405968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8117,7 +8118,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348537840"/>
+        <c:crossAx val="455407928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8125,7 +8126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348537840"/>
+        <c:axId val="455407928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8176,7 +8177,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348536664"/>
+        <c:crossAx val="455405968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8594,11 +8595,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348539016"/>
-        <c:axId val="348537056"/>
+        <c:axId val="455405184"/>
+        <c:axId val="455405576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348539016"/>
+        <c:axId val="455405184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8641,7 +8642,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348537056"/>
+        <c:crossAx val="455405576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8649,7 +8650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348537056"/>
+        <c:axId val="455405576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8700,7 +8701,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348539016"/>
+        <c:crossAx val="455405184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9109,11 +9110,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348538232"/>
-        <c:axId val="348538624"/>
+        <c:axId val="455406752"/>
+        <c:axId val="455407144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348538232"/>
+        <c:axId val="455406752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9156,7 +9157,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348538624"/>
+        <c:crossAx val="455407144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9164,7 +9165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348538624"/>
+        <c:axId val="455407144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9215,7 +9216,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348538232"/>
+        <c:crossAx val="455406752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9624,11 +9625,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348539800"/>
-        <c:axId val="348540976"/>
+        <c:axId val="448769144"/>
+        <c:axId val="448764832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348539800"/>
+        <c:axId val="448769144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9671,7 +9672,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348540976"/>
+        <c:crossAx val="448764832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9679,7 +9680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348540976"/>
+        <c:axId val="448764832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9730,7 +9731,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348539800"/>
+        <c:crossAx val="448769144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10090,11 +10091,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="348540192"/>
-        <c:axId val="136534696"/>
+        <c:axId val="448776984"/>
+        <c:axId val="448774632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348540192"/>
+        <c:axId val="448776984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10137,7 +10138,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136534696"/>
+        <c:crossAx val="448774632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10145,7 +10146,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136534696"/>
+        <c:axId val="448774632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10196,7 +10197,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348540192"/>
+        <c:crossAx val="448776984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10547,11 +10548,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="136528816"/>
-        <c:axId val="136532736"/>
+        <c:axId val="448765616"/>
+        <c:axId val="448767968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136528816"/>
+        <c:axId val="448765616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10594,7 +10595,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136532736"/>
+        <c:crossAx val="448767968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10602,7 +10603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136532736"/>
+        <c:axId val="448767968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10653,7 +10654,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136528816"/>
+        <c:crossAx val="448765616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11004,11 +11005,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="136533912"/>
-        <c:axId val="136528424"/>
+        <c:axId val="448771888"/>
+        <c:axId val="448768752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136533912"/>
+        <c:axId val="448771888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11051,7 +11052,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136528424"/>
+        <c:crossAx val="448768752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11059,7 +11060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136528424"/>
+        <c:axId val="448768752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11110,7 +11111,654 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136533912"/>
+        <c:crossAx val="448771888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1000"/>
+              <a:t>Comparisons</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1000" baseline="0"/>
+              <a:t> with another normalisation </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1000" baseline="0"/>
+              <a:t>(minus nlogn and then divided by n) </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Tabelle1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reinhardt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$O$59:$O$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-0.11478428466208788</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.6970123795494495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.76653047443681166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.76618856932417301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.78343896421153847</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.7444724590989017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.78437487798626326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B760-43C3-8DCC-2AE83CF94139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Tabelle1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$P$59:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.82121571533791216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.31001237954944955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.74901047443681168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.92369156932417307</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.96450106421153847</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.98623519909890178</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.0010840589862633</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B760-43C3-8DCC-2AE83CF94139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Tabelle1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Huang/Langston</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$Q$59:$Q$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.59421571533791206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14438762045055045</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.12044047443681163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.21293056932417304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.22560026421153842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.24078321909890174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.25125393198626328</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B760-43C3-8DCC-2AE83CF94139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Tabelle1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdStableSort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$A$11:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Tabelle1!$R$59:$R$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-0.20378428466208789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.5105123795494495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.65594047443681158</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.10882056932417303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.5108832642115384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.61714966909890179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0737800137367245E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B760-43C3-8DCC-2AE83CF94139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="446924520"/>
+        <c:axId val="448610224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="446924520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448610224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="448610224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446924520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11638,11 +12286,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="346766944"/>
-        <c:axId val="346770080"/>
+        <c:axId val="449524728"/>
+        <c:axId val="449531000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346766944"/>
+        <c:axId val="449524728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11685,7 +12333,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346770080"/>
+        <c:crossAx val="449531000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11693,7 +12341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346770080"/>
+        <c:axId val="449531000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11744,7 +12392,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346766944"/>
+        <c:crossAx val="449524728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12257,11 +12905,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="346767336"/>
-        <c:axId val="346767728"/>
+        <c:axId val="449528256"/>
+        <c:axId val="449525120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346767336"/>
+        <c:axId val="449528256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12304,7 +12952,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346767728"/>
+        <c:crossAx val="449525120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12312,7 +12960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346767728"/>
+        <c:axId val="449525120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12363,7 +13011,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346767336"/>
+        <c:crossAx val="449528256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12876,11 +13524,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="346769688"/>
-        <c:axId val="346768120"/>
+        <c:axId val="449523552"/>
+        <c:axId val="449530608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346769688"/>
+        <c:axId val="449523552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12923,7 +13571,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346768120"/>
+        <c:crossAx val="449530608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12931,7 +13579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346768120"/>
+        <c:axId val="449530608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12982,7 +13630,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346769688"/>
+        <c:crossAx val="449523552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13495,11 +14143,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="346769296"/>
-        <c:axId val="347273232"/>
+        <c:axId val="449523944"/>
+        <c:axId val="449529432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346769296"/>
+        <c:axId val="449523944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13542,7 +14190,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347273232"/>
+        <c:crossAx val="449529432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13550,7 +14198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347273232"/>
+        <c:axId val="449529432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13601,7 +14249,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346769296"/>
+        <c:crossAx val="449523944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14014,11 +14662,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347274800"/>
-        <c:axId val="347270880"/>
+        <c:axId val="449525512"/>
+        <c:axId val="449532176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347274800"/>
+        <c:axId val="449525512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14061,7 +14709,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347270880"/>
+        <c:crossAx val="449532176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14069,7 +14717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347270880"/>
+        <c:axId val="449532176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14120,7 +14768,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347274800"/>
+        <c:crossAx val="449525512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14533,11 +15181,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347274016"/>
-        <c:axId val="347270488"/>
+        <c:axId val="449526688"/>
+        <c:axId val="449531392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347274016"/>
+        <c:axId val="449526688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14580,7 +15228,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347270488"/>
+        <c:crossAx val="449531392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14588,7 +15236,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347270488"/>
+        <c:axId val="449531392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14639,7 +15287,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347274016"/>
+        <c:crossAx val="449526688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -15053,11 +15701,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347273624"/>
-        <c:axId val="347275976"/>
+        <c:axId val="449531784"/>
+        <c:axId val="449532568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347273624"/>
+        <c:axId val="449531784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15100,7 +15748,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347275976"/>
+        <c:crossAx val="449532568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15108,7 +15756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347275976"/>
+        <c:axId val="449532568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15159,7 +15807,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347273624"/>
+        <c:crossAx val="449531784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -16081,6 +16729,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -26924,6 +27612,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -30465,7 +31656,7 @@
         <xdr:cNvPr id="5" name="Diagramm 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30501,7 +31692,7 @@
         <xdr:cNvPr id="9" name="Diagramm 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30539,7 +31730,7 @@
         <xdr:cNvPr id="10" name="Diagramm 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30577,7 +31768,7 @@
         <xdr:cNvPr id="13" name="Diagramm 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30615,7 +31806,7 @@
         <xdr:cNvPr id="15" name="Diagramm 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30653,7 +31844,7 @@
         <xdr:cNvPr id="17" name="Diagramm 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30691,7 +31882,7 @@
         <xdr:cNvPr id="12" name="Diagramm 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30729,7 +31920,7 @@
         <xdr:cNvPr id="18" name="Diagramm 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30767,7 +31958,7 @@
         <xdr:cNvPr id="21" name="Diagramm 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30805,7 +31996,7 @@
         <xdr:cNvPr id="22" name="Diagramm 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30843,7 +32034,7 @@
         <xdr:cNvPr id="27" name="Diagramm 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30881,7 +32072,7 @@
         <xdr:cNvPr id="29" name="Diagramm 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30919,7 +32110,7 @@
         <xdr:cNvPr id="32" name="Diagramm 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30957,7 +32148,7 @@
         <xdr:cNvPr id="34" name="Diagramm 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30995,7 +32186,7 @@
         <xdr:cNvPr id="36" name="Diagramm 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31033,7 +32224,7 @@
         <xdr:cNvPr id="26" name="Diagramm 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31071,7 +32262,7 @@
         <xdr:cNvPr id="28" name="Diagramm 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31109,7 +32300,7 @@
         <xdr:cNvPr id="30" name="Diagramm 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31147,7 +32338,7 @@
         <xdr:cNvPr id="39" name="Diagramm 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31185,7 +32376,7 @@
         <xdr:cNvPr id="41" name="Diagramm 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31223,7 +32414,7 @@
         <xdr:cNvPr id="44" name="Diagramm 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31261,7 +32452,7 @@
         <xdr:cNvPr id="46" name="Diagramm 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31299,7 +32490,7 @@
         <xdr:cNvPr id="48" name="Diagramm 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31337,7 +32528,7 @@
         <xdr:cNvPr id="43" name="Diagramm 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31375,7 +32566,7 @@
         <xdr:cNvPr id="50" name="Diagramm 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000032000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31413,7 +32604,7 @@
         <xdr:cNvPr id="49" name="Diagramm 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31451,7 +32642,7 @@
         <xdr:cNvPr id="57" name="Diagramm 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000039000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31489,7 +32680,7 @@
         <xdr:cNvPr id="58" name="Diagramm 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31509,7 +32700,206 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>604555</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>71695</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="31" name="Diagramm 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Reinhardt</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Chen</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Huang/Langston</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>StdStableSort</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1000</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>10000</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>100000</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>1000000</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>10000000</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>100000000</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>1000000000</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="O59">
+            <v>-0.11478428466208788</v>
+          </cell>
+          <cell r="P59">
+            <v>0.82121571533791216</v>
+          </cell>
+          <cell r="Q59">
+            <v>0.59421571533791206</v>
+          </cell>
+          <cell r="R59">
+            <v>-0.20378428466208789</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="O60">
+            <v>-0.6970123795494495</v>
+          </cell>
+          <cell r="P60">
+            <v>-0.31001237954944955</v>
+          </cell>
+          <cell r="Q60">
+            <v>0.14438762045055045</v>
+          </cell>
+          <cell r="R60">
+            <v>-0.5105123795494495</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="O61">
+            <v>-0.76653047443681166</v>
+          </cell>
+          <cell r="P61">
+            <v>-0.74901047443681168</v>
+          </cell>
+          <cell r="Q61">
+            <v>-0.12044047443681163</v>
+          </cell>
+          <cell r="R61">
+            <v>-0.65594047443681158</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="O62">
+            <v>-0.76618856932417301</v>
+          </cell>
+          <cell r="P62">
+            <v>-0.92369156932417307</v>
+          </cell>
+          <cell r="Q62">
+            <v>-0.21293056932417304</v>
+          </cell>
+          <cell r="R62">
+            <v>-0.10882056932417303</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="O63">
+            <v>-0.78343896421153847</v>
+          </cell>
+          <cell r="P63">
+            <v>-0.96450106421153847</v>
+          </cell>
+          <cell r="Q63">
+            <v>-0.22560026421153842</v>
+          </cell>
+          <cell r="R63">
+            <v>-0.5108832642115384</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="O64">
+            <v>-0.7444724590989017</v>
+          </cell>
+          <cell r="P64">
+            <v>-0.98623519909890178</v>
+          </cell>
+          <cell r="Q64">
+            <v>-0.24078321909890174</v>
+          </cell>
+          <cell r="R64">
+            <v>-0.61714966909890179</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="O65">
+            <v>-0.78437487798626326</v>
+          </cell>
+          <cell r="P65">
+            <v>-1.0010840589862633</v>
+          </cell>
+          <cell r="Q65">
+            <v>-0.25125393198626328</v>
+          </cell>
+          <cell r="R65">
+            <v>8.0737800137367245E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31777,8 +33167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q143" sqref="Q143"/>
+    <sheetView tabSelected="1" topLeftCell="K36" zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC56" sqref="AC56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32691,7 +34081,7 @@
         <v>21856973</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>10000000</v>
       </c>
@@ -32707,8 +34097,23 @@
       <c r="E49" s="1">
         <v>238571223</v>
       </c>
+      <c r="N49" s="3">
+        <v>1000</v>
+      </c>
+      <c r="O49">
+        <v>9851</v>
+      </c>
+      <c r="P49">
+        <v>10787</v>
+      </c>
+      <c r="Q49">
+        <v>10560</v>
+      </c>
+      <c r="R49">
+        <v>9762</v>
+      </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A50" s="3">
         <v>100000000</v>
       </c>
@@ -32724,8 +34129,23 @@
       <c r="E50" s="1">
         <v>2785718657</v>
       </c>
+      <c r="N50" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O50">
+        <v>125907</v>
+      </c>
+      <c r="P50">
+        <v>129777</v>
+      </c>
+      <c r="Q50">
+        <v>134321</v>
+      </c>
+      <c r="R50">
+        <v>127772</v>
+      </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>1000000000</v>
       </c>
@@ -32741,17 +34161,77 @@
       <c r="E51" s="1">
         <v>31857174641</v>
       </c>
+      <c r="N51" s="3">
+        <v>100000</v>
+      </c>
+      <c r="O51">
+        <v>1584311</v>
+      </c>
+      <c r="P51">
+        <v>1586063</v>
+      </c>
+      <c r="Q51">
+        <v>1648920</v>
+      </c>
+      <c r="R51">
+        <v>1595370</v>
+      </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E52" s="1"/>
+      <c r="N52" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="O52">
+        <v>19165380</v>
+      </c>
+      <c r="P52">
+        <v>19007877</v>
+      </c>
+      <c r="Q52">
+        <v>19718638</v>
+      </c>
+      <c r="R52">
+        <v>19822748</v>
+      </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E53" s="1"/>
+      <c r="N53" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="O53">
+        <v>224700577</v>
+      </c>
+      <c r="P53">
+        <v>222889956</v>
+      </c>
+      <c r="Q53">
+        <v>230278964</v>
+      </c>
+      <c r="R53">
+        <v>227426134</v>
+      </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E54" s="1"/>
+      <c r="N54" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="O54">
+        <v>2583095230</v>
+      </c>
+      <c r="P54">
+        <v>2558918956</v>
+      </c>
+      <c r="Q54">
+        <v>2633464154</v>
+      </c>
+      <c r="R54">
+        <v>2595827509</v>
+      </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>1000</v>
       </c>
@@ -32771,8 +34251,23 @@
         <f xml:space="preserve"> E45/ (A45*LOG(A45, 2))</f>
         <v>1.1889681395408376</v>
       </c>
+      <c r="N55" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="O55">
+        <v>29112977976</v>
+      </c>
+      <c r="P55">
+        <v>28896268795</v>
+      </c>
+      <c r="Q55">
+        <v>29646098922</v>
+      </c>
+      <c r="R55">
+        <v>29905426634</v>
+      </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>10000</v>
       </c>
@@ -32793,7 +34288,7 @@
         <v>1.0427904822297056</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>100000</v>
       </c>
@@ -32814,7 +34309,7 @@
         <v>1.0750894956144725</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>1000000</v>
       </c>
@@ -32835,7 +34330,7 @@
         <v>1.0966007479029591</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>10000000</v>
       </c>
@@ -32855,8 +34350,27 @@
         <f t="shared" si="15"/>
         <v>1.0259584889320097</v>
       </c>
+      <c r="N59" s="3">
+        <v>1000</v>
+      </c>
+      <c r="O59" s="3">
+        <f>(O49 - (N49*LOG(N49, 2))) / N49</f>
+        <v>-0.11478428466208788</v>
+      </c>
+      <c r="P59" s="3">
+        <f>(P49 - (N49*LOG(N49, 2))) / N49</f>
+        <v>0.82121571533791216</v>
+      </c>
+      <c r="Q59" s="3">
+        <f>(Q49 - (N49*LOG(N49, 2))) / N49</f>
+        <v>0.59421571533791206</v>
+      </c>
+      <c r="R59" s="3">
+        <f>(R49 - (N49*LOG(N49, 2))) / N49</f>
+        <v>-0.20378428466208789</v>
+      </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>100000000</v>
       </c>
@@ -32876,8 +34390,27 @@
         <f t="shared" si="15"/>
         <v>1.0482310940472268</v>
       </c>
+      <c r="N60" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O60" s="3">
+        <f t="shared" ref="O60:O65" si="16">(O50 - (N50*LOG(N50, 2))) / N50</f>
+        <v>-0.6970123795494495</v>
+      </c>
+      <c r="P60" s="3">
+        <f t="shared" ref="P60:P65" si="17">(P50 - (N50*LOG(N50, 2))) / N50</f>
+        <v>-0.31001237954944955</v>
+      </c>
+      <c r="Q60" s="3">
+        <f t="shared" ref="Q60:Q65" si="18">(Q50 - (N50*LOG(N50, 2))) / N50</f>
+        <v>0.14438762045055045</v>
+      </c>
+      <c r="R60" s="3">
+        <f t="shared" ref="R60:R65" si="19">(R50 - (N50*LOG(N50, 2))) / N50</f>
+        <v>-0.5105123795494495</v>
+      </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>1000000000</v>
       </c>
@@ -32897,26 +34430,121 @@
         <f t="shared" si="15"/>
         <v>1.0655516826718801</v>
       </c>
+      <c r="N61" s="3">
+        <v>100000</v>
+      </c>
+      <c r="O61" s="3">
+        <f t="shared" si="16"/>
+        <v>-0.76653047443681166</v>
+      </c>
+      <c r="P61" s="3">
+        <f t="shared" si="17"/>
+        <v>-0.74901047443681168</v>
+      </c>
+      <c r="Q61" s="3">
+        <f t="shared" si="18"/>
+        <v>-0.12044047443681163</v>
+      </c>
+      <c r="R61" s="3">
+        <f t="shared" si="19"/>
+        <v>-0.65594047443681158</v>
+      </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E62" s="1"/>
+      <c r="N62" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="O62" s="3">
+        <f t="shared" si="16"/>
+        <v>-0.76618856932417301</v>
+      </c>
+      <c r="P62" s="3">
+        <f t="shared" si="17"/>
+        <v>-0.92369156932417307</v>
+      </c>
+      <c r="Q62" s="3">
+        <f t="shared" si="18"/>
+        <v>-0.21293056932417304</v>
+      </c>
+      <c r="R62" s="3">
+        <f t="shared" si="19"/>
+        <v>-0.10882056932417303</v>
+      </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E63" s="1"/>
+      <c r="N63" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="O63" s="3">
+        <f t="shared" si="16"/>
+        <v>-0.78343896421153847</v>
+      </c>
+      <c r="P63" s="3">
+        <f t="shared" si="17"/>
+        <v>-0.96450106421153847</v>
+      </c>
+      <c r="Q63" s="3">
+        <f t="shared" si="18"/>
+        <v>-0.22560026421153842</v>
+      </c>
+      <c r="R63" s="3">
+        <f t="shared" si="19"/>
+        <v>-0.5108832642115384</v>
+      </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E64" s="1"/>
+      <c r="N64" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="O64" s="3">
+        <f t="shared" si="16"/>
+        <v>-0.7444724590989017</v>
+      </c>
+      <c r="P64" s="3">
+        <f t="shared" si="17"/>
+        <v>-0.98623519909890178</v>
+      </c>
+      <c r="Q64" s="3">
+        <f t="shared" si="18"/>
+        <v>-0.24078321909890174</v>
+      </c>
+      <c r="R64" s="3">
+        <f t="shared" si="19"/>
+        <v>-0.61714966909890179</v>
+      </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E65" s="1"/>
+      <c r="N65" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="O65" s="3">
+        <f t="shared" si="16"/>
+        <v>-0.78437487798626326</v>
+      </c>
+      <c r="P65" s="3">
+        <f t="shared" si="17"/>
+        <v>-1.0010840589862633</v>
+      </c>
+      <c r="Q65" s="3">
+        <f t="shared" si="18"/>
+        <v>-0.25125393198626328</v>
+      </c>
+      <c r="R65" s="3">
+        <f t="shared" si="19"/>
+        <v>8.0737800137367245E-3</v>
+      </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A68" s="3">
         <v>1000</v>
       </c>
@@ -32933,7 +34561,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>10000</v>
       </c>
@@ -32950,7 +34578,7 @@
         <v>10412</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A70" s="3">
         <v>100000</v>
       </c>
@@ -32967,7 +34595,7 @@
         <v>131611</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A71" s="3">
         <v>1000000</v>
       </c>
@@ -32984,7 +34612,7 @@
         <v>1662230</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A72" s="3">
         <v>10000000</v>
       </c>
@@ -33001,13 +34629,13 @@
         <v>18483295</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A75" s="3">
         <v>1000</v>
       </c>
@@ -33028,91 +34656,91 @@
         <v>8.1177755497386928E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A76" s="3">
         <v>10000</v>
       </c>
       <c r="B76" s="2">
-        <f t="shared" ref="B76:B79" si="16" xml:space="preserve"> B69/ (A69*LOG(A69, 2))</f>
+        <f t="shared" ref="B76:B79" si="20" xml:space="preserve"> B69/ (A69*LOG(A69, 2))</f>
         <v>0.1168146898174079</v>
       </c>
       <c r="C76" s="2">
-        <f t="shared" ref="C76:C79" si="17" xml:space="preserve"> C69/ (A69*LOG(A69, 2))</f>
+        <f t="shared" ref="C76:C79" si="21" xml:space="preserve"> C69/ (A69*LOG(A69, 2))</f>
         <v>0.11342057661629651</v>
       </c>
       <c r="D76" s="2">
-        <f t="shared" ref="D76:D79" si="18" xml:space="preserve"> D69/ (A69*LOG(A69, 2))</f>
+        <f t="shared" ref="D76:D79" si="22" xml:space="preserve"> D69/ (A69*LOG(A69, 2))</f>
         <v>0.12098395525735404</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" ref="E76:E79" si="19" xml:space="preserve"> E69/ (A69*LOG(A69, 2))</f>
+        <f t="shared" ref="E76:E79" si="23" xml:space="preserve"> E69/ (A69*LOG(A69, 2))</f>
         <v>7.8358107871334307E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A77" s="3">
         <v>100000</v>
       </c>
       <c r="B77" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.11996767799199244</v>
       </c>
       <c r="C77" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.11917476498341352</v>
       </c>
       <c r="D77" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.12785647005836273</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7.9237717518664458E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A78" s="3">
         <v>1000000</v>
       </c>
       <c r="B78" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.12252091407188245</v>
       </c>
       <c r="C78" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.11158750462936665</v>
       </c>
       <c r="D78" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.11917491549841136</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>8.3396848282089917E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A79" s="3">
         <v>10000000</v>
       </c>
       <c r="B79" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.11649294895804223</v>
       </c>
       <c r="C79" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.11252595417303973</v>
       </c>
       <c r="D79" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.11967263849324217</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7.948608876722979E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
@@ -33241,19 +34869,19 @@
         <v>10000</v>
       </c>
       <c r="B92" s="2">
-        <f t="shared" ref="B92:B95" si="20">B85/ (A85*LOG(A85, 2))</f>
+        <f t="shared" ref="B92:B95" si="24">B85/ (A85*LOG(A85, 2))</f>
         <v>7.7695841880873542E-2</v>
       </c>
       <c r="C92" s="2">
-        <f t="shared" ref="C92:C95" si="21">C85/ (A85*LOG(A85, 2))</f>
+        <f t="shared" ref="C92:C95" si="25">C85/ (A85*LOG(A85, 2))</f>
         <v>7.5438116913393694E-2</v>
       </c>
       <c r="D92" s="2">
-        <f t="shared" ref="D92:D95" si="22">D85/ (A85*LOG(A85, 2))</f>
+        <f t="shared" ref="D92:D95" si="26">D85/ (A85*LOG(A85, 2))</f>
         <v>8.2896135055968823E-2</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" ref="E92:E95" si="23">E85/ (A85*LOG(A85, 2))</f>
+        <f t="shared" ref="E92:E95" si="27">E85/ (A85*LOG(A85, 2))</f>
         <v>4.8510983801250566E-2</v>
       </c>
     </row>
@@ -33262,19 +34890,19 @@
         <v>100000</v>
       </c>
       <c r="B93" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.1332284228494436E-2</v>
       </c>
       <c r="C93" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7.8870460923954402E-2</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>8.5685177965795611E-2</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>5.1179313682816099E-2</v>
       </c>
     </row>
@@ -33283,19 +34911,19 @@
         <v>1000000</v>
       </c>
       <c r="B94" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.263524239306004E-2</v>
       </c>
       <c r="C94" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7.7808477270917817E-2</v>
       </c>
       <c r="D94" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>8.4863867794292377E-2</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>5.4589080443702018E-2</v>
       </c>
     </row>
@@ -33304,19 +34932,19 @@
         <v>10000000</v>
       </c>
       <c r="B95" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.1834630183972953E-2</v>
       </c>
       <c r="C95" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7.9159802354929601E-2</v>
       </c>
       <c r="D95" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>8.5174041934443695E-2</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>5.0953657297637865E-2</v>
       </c>
     </row>
@@ -33443,19 +35071,19 @@
         <v>10000</v>
       </c>
       <c r="B106" s="2">
-        <f t="shared" ref="B106:B109" si="24">B99/ (A99*LOG(A99, 2))</f>
+        <f t="shared" ref="B106:B109" si="28">B99/ (A99*LOG(A99, 2))</f>
         <v>5.7474151922145611E-2</v>
       </c>
       <c r="C106" s="2">
-        <f t="shared" ref="C106:C109" si="25">C99/ (A99*LOG(A99, 2))</f>
+        <f t="shared" ref="C106:C109" si="29">C99/ (A99*LOG(A99, 2))</f>
         <v>6.0010329635614652E-2</v>
       </c>
       <c r="D106" s="2">
-        <f t="shared" ref="D106:D109" si="26">D99/ (A99*LOG(A99, 2))</f>
+        <f t="shared" ref="D106:D109" si="30">D99/ (A99*LOG(A99, 2))</f>
         <v>5.6397969687646876E-2</v>
       </c>
       <c r="E106" s="1">
-        <f t="shared" ref="E106:E109" si="27">E99/ (A99*LOG(A99, 2))</f>
+        <f t="shared" ref="E106:E109" si="31">E99/ (A99*LOG(A99, 2))</f>
         <v>4.6162949835071514E-2</v>
       </c>
     </row>
@@ -33464,19 +35092,19 @@
         <v>100000</v>
       </c>
       <c r="B107" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6.0428761329587584E-2</v>
       </c>
       <c r="C107" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>6.5792513792328408E-2</v>
       </c>
       <c r="D107" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>6.3648578163209527E-2</v>
       </c>
       <c r="E107" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>4.9086553152960101E-2</v>
       </c>
     </row>
@@ -33485,19 +35113,19 @@
         <v>1000000</v>
       </c>
       <c r="B108" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.6552730644005529E-2</v>
       </c>
       <c r="C108" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>7.4677514457682698E-2</v>
       </c>
       <c r="D108" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>7.3541276739049005E-2</v>
       </c>
       <c r="E108" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.8736719031841396E-2</v>
       </c>
     </row>
@@ -33506,19 +35134,19 @@
         <v>10000000</v>
       </c>
       <c r="B109" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.5502254938716132E-2</v>
       </c>
       <c r="C109" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>8.6647188123796001E-2</v>
       </c>
       <c r="D109" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.7335901749590092E-2</v>
       </c>
       <c r="E109" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>9.5201553210150849E-2</v>
       </c>
     </row>
@@ -33608,19 +35236,19 @@
         <v>10000000</v>
       </c>
       <c r="B125" s="2">
-        <f t="shared" ref="B125:B126" si="28" xml:space="preserve"> B120/ (A120*LOG(A120, 2))</f>
+        <f t="shared" ref="B125:B126" si="32" xml:space="preserve"> B120/ (A120*LOG(A120, 2))</f>
         <v>8.3081225499017069E-3</v>
       </c>
       <c r="C125" s="2">
-        <f t="shared" ref="C125:C126" si="29" xml:space="preserve"> C120/ (A120*LOG(A120, 2))</f>
+        <f t="shared" ref="C125:C126" si="33" xml:space="preserve"> C120/ (A120*LOG(A120, 2))</f>
         <v>8.3152010552283197E-3</v>
       </c>
       <c r="D125" s="2">
-        <f t="shared" ref="D125:D126" si="30" xml:space="preserve"> D120/ (A120*LOG(A120, 2))</f>
+        <f t="shared" ref="D125:D126" si="34" xml:space="preserve"> D120/ (A120*LOG(A120, 2))</f>
         <v>8.3828295939684886E-3</v>
       </c>
       <c r="E125" s="1">
-        <f t="shared" ref="E125:E126" si="31" xml:space="preserve"> E120/ (A120*LOG(A120, 2))</f>
+        <f t="shared" ref="E125:E126" si="35" xml:space="preserve"> E120/ (A120*LOG(A120, 2))</f>
         <v>8.5249716574925111E-3</v>
       </c>
     </row>
@@ -33629,19 +35257,19 @@
         <v>100000000</v>
       </c>
       <c r="B126" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>8.5063709065497199E-3</v>
       </c>
       <c r="C126" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>8.5552088841837608E-3</v>
       </c>
       <c r="D126" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>8.5801300286622983E-3</v>
       </c>
       <c r="E126" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>8.6919205278520734E-3</v>
       </c>
     </row>
@@ -33737,19 +35365,19 @@
         <v>10000000</v>
       </c>
       <c r="B138" s="2">
-        <f t="shared" ref="B138:B139" si="32">B130/ (A130*LOG(A130, 2))</f>
+        <f t="shared" ref="B138:B139" si="36">B130/ (A130*LOG(A130, 2))</f>
         <v>1.1739044580771474</v>
       </c>
       <c r="C138" s="2">
-        <f t="shared" ref="C138:C139" si="33">C130/ (A130*LOG(A130, 2))</f>
+        <f t="shared" ref="C138:C139" si="37">C130/ (A130*LOG(A130, 2))</f>
         <v>1.1492448635103427</v>
       </c>
       <c r="D138" s="2">
-        <f t="shared" ref="D138:D139" si="34">D130/ (A130*LOG(A130, 2))</f>
+        <f t="shared" ref="D138:D139" si="38">D130/ (A130*LOG(A130, 2))</f>
         <v>1.1570563080695415</v>
       </c>
       <c r="E138" s="1">
-        <f t="shared" ref="E138:E139" si="35">E130/ (A130*LOG(A130, 2))</f>
+        <f t="shared" ref="E138:E139" si="39">E130/ (A130*LOG(A130, 2))</f>
         <v>1.1572537407424119</v>
       </c>
     </row>
@@ -33758,19 +35386,19 @@
         <v>100000000</v>
       </c>
       <c r="B139" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>1.1916357257528847</v>
       </c>
       <c r="C139" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>1.1914624954078674</v>
       </c>
       <c r="D139" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1.1775391552033683</v>
       </c>
       <c r="E139" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1.1722730045672591</v>
       </c>
     </row>
@@ -33885,15 +35513,15 @@
         <v>2.0946664238658306</v>
       </c>
       <c r="C154" s="2">
-        <f t="shared" ref="C154:C155" si="36">C149/ (A149*LOG(A149, 2))</f>
+        <f t="shared" ref="C154:C155" si="40">C149/ (A149*LOG(A149, 2))</f>
         <v>2.1113001717096673</v>
       </c>
       <c r="D154" s="2">
-        <f t="shared" ref="D154:D155" si="37">D149/ (A149*LOG(A149, 2))</f>
+        <f t="shared" ref="D154:D155" si="41">D149/ (A149*LOG(A149, 2))</f>
         <v>2.3762514514663242</v>
       </c>
       <c r="E154" s="1">
-        <f t="shared" ref="E154:E155" si="38">E149/ (A149*LOG(A149, 2))</f>
+        <f t="shared" ref="E154:E155" si="42">E149/ (A149*LOG(A149, 2))</f>
         <v>2.5350767349637571</v>
       </c>
     </row>
@@ -33902,19 +35530,19 @@
         <v>100000000</v>
       </c>
       <c r="B155" s="2">
-        <f t="shared" ref="B155" si="39">B150/ (A150*LOG(A150, 2))</f>
+        <f t="shared" ref="B155" si="43">B150/ (A150*LOG(A150, 2))</f>
         <v>2.1464053672545749</v>
       </c>
       <c r="C155" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.1722506994073503</v>
       </c>
       <c r="D155" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>2.3930696738243364</v>
       </c>
       <c r="E155" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>2.5189219809960171</v>
       </c>
     </row>
@@ -34025,19 +35653,19 @@
         <v>10000000</v>
       </c>
       <c r="B170" s="2">
-        <f t="shared" ref="B170:B171" si="40">B165/ (A165*LOG(A165, 2))</f>
+        <f t="shared" ref="B170:B171" si="44">B165/ (A165*LOG(A165, 2))</f>
         <v>8.1857280540932418E-3</v>
       </c>
       <c r="C170" s="2">
-        <f t="shared" ref="C170:C171" si="41">C165/ (A165*LOG(A165, 2))</f>
+        <f t="shared" ref="C170:C171" si="45">C165/ (A165*LOG(A165, 2))</f>
         <v>1.0630513060878699E-2</v>
       </c>
       <c r="D170" s="2">
-        <f t="shared" ref="D170:D171" si="42">D165/ (A165*LOG(A165, 2))</f>
+        <f t="shared" ref="D170:D171" si="46">D165/ (A165*LOG(A165, 2))</f>
         <v>8.3168008146338492E-3</v>
       </c>
       <c r="E170" s="1">
-        <f t="shared" ref="E170:E171" si="43">E165/ (A165*LOG(A165, 2))</f>
+        <f t="shared" ref="E170:E171" si="47">E165/ (A165*LOG(A165, 2))</f>
         <v>9.5560466973552503E-3</v>
       </c>
     </row>
@@ -34046,19 +35674,19 @@
         <v>100000000</v>
       </c>
       <c r="B171" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>8.3761995158247015E-3</v>
       </c>
       <c r="C171" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>1.098686258627086E-2</v>
       </c>
       <c r="D171" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>8.4924565475751421E-3</v>
       </c>
       <c r="E171" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>9.8761962369063351E-3</v>
       </c>
     </row>
@@ -34172,19 +35800,19 @@
         <v>10000000</v>
       </c>
       <c r="B187" s="2">
-        <f t="shared" ref="B187:B188" si="44">B182/ (A182*LOG(A182, 2))</f>
+        <f t="shared" ref="B187:B188" si="48">B182/ (A182*LOG(A182, 2))</f>
         <v>1.1829976625553122</v>
       </c>
       <c r="C187" s="2">
-        <f t="shared" ref="C187:C188" si="45">C182/ (A182*LOG(A182, 2))</f>
+        <f t="shared" ref="C187:C188" si="49">C182/ (A182*LOG(A182, 2))</f>
         <v>1.6125603104547737</v>
       </c>
       <c r="D187" s="2">
-        <f t="shared" ref="D187:D188" si="46">D182/ (A182*LOG(A182, 2))</f>
+        <f t="shared" ref="D187:D188" si="50">D182/ (A182*LOG(A182, 2))</f>
         <v>1.1720352424220715</v>
       </c>
       <c r="E187" s="1">
-        <f t="shared" ref="E187:E188" si="47">E182/ (A182*LOG(A182, 2))</f>
+        <f t="shared" ref="E187:E188" si="51">E182/ (A182*LOG(A182, 2))</f>
         <v>1.153062818344492</v>
       </c>
     </row>
@@ -34193,19 +35821,19 @@
         <v>100000000</v>
       </c>
       <c r="B188" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>1.1988503216337785</v>
       </c>
       <c r="C188" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>1.6515562982666026</v>
       </c>
       <c r="D188" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>1.1892453767527902</v>
       </c>
       <c r="E188" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>1.1729574801745126</v>
       </c>
     </row>
@@ -34313,19 +35941,19 @@
         <v>10000000</v>
       </c>
       <c r="B202" s="2">
-        <f t="shared" ref="B202:B203" si="48">B197/ (A197*LOG(A197, 2))</f>
+        <f t="shared" ref="B202:B203" si="52">B197/ (A197*LOG(A197, 2))</f>
         <v>2.0937663054749387</v>
       </c>
       <c r="C202" s="2">
-        <f t="shared" ref="C202:C203" si="49">C197/ (A197*LOG(A197, 2))</f>
+        <f t="shared" ref="C202:C203" si="53">C197/ (A197*LOG(A197, 2))</f>
         <v>4.4162144550952425</v>
       </c>
       <c r="D202" s="2">
-        <f t="shared" ref="D202:D203" si="50">D197/ (A197*LOG(A197, 2))</f>
+        <f t="shared" ref="D202:D203" si="54">D197/ (A197*LOG(A197, 2))</f>
         <v>2.0937754051816646</v>
       </c>
       <c r="E202" s="1">
-        <f t="shared" ref="E202:E203" si="51">E197/ (A197*LOG(A197, 2))</f>
+        <f t="shared" ref="E202:E203" si="55">E197/ (A197*LOG(A197, 2))</f>
         <v>4.419182099101497</v>
       </c>
     </row>
@@ -34334,19 +35962,19 @@
         <v>100000000</v>
       </c>
       <c r="B203" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>2.1455384625782119</v>
       </c>
       <c r="C203" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>4.5588035494529544</v>
       </c>
       <c r="D203" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>2.1454748263422783</v>
       </c>
       <c r="E203" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>4.559974079379832</v>
       </c>
     </row>
@@ -34460,19 +36088,19 @@
         <v>10000000</v>
       </c>
       <c r="B219" s="2">
-        <f t="shared" ref="B219:B220" si="52">B214/ (A214*LOG(A214, 2))</f>
+        <f t="shared" ref="B219:B220" si="56">B214/ (A214*LOG(A214, 2))</f>
         <v>8.4345121437954841E-3</v>
       </c>
       <c r="C219" s="2">
-        <f t="shared" ref="C219:C220" si="53">C214/ (A214*LOG(A214, 2))</f>
+        <f t="shared" ref="C219:C220" si="57">C214/ (A214*LOG(A214, 2))</f>
         <v>8.4910885812662738E-3</v>
       </c>
       <c r="D219" s="2">
-        <f t="shared" ref="D219:D220" si="54">D214/ (A214*LOG(A214, 2))</f>
+        <f t="shared" ref="D219:D220" si="58">D214/ (A214*LOG(A214, 2))</f>
         <v>8.1143237391217444E-3</v>
       </c>
       <c r="E219" s="1">
-        <f t="shared" ref="E219:E220" si="55">E214/ (A214*LOG(A214, 2))</f>
+        <f t="shared" ref="E219:E220" si="59">E214/ (A214*LOG(A214, 2))</f>
         <v>8.1246748705440762E-3</v>
       </c>
     </row>
@@ -34481,19 +36109,19 @@
         <v>100000000</v>
       </c>
       <c r="B220" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>8.4564684115935127E-3</v>
       </c>
       <c r="C220" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>8.4959947788866771E-3</v>
       </c>
       <c r="D220" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>8.2580350827642351E-3</v>
       </c>
       <c r="E220" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>8.296416030923898E-3</v>
       </c>
     </row>
@@ -34598,19 +36226,19 @@
         <v>10000000</v>
       </c>
       <c r="B233" s="2">
-        <f t="shared" ref="B233:B234" si="56">B228/ (A228*LOG(A228, 2))</f>
+        <f t="shared" ref="B233:B234" si="60">B228/ (A228*LOG(A228, 2))</f>
         <v>0.96350964001394801</v>
       </c>
       <c r="C233" s="2">
-        <f t="shared" ref="C233:C234" si="57">C228/ (A228*LOG(A228, 2))</f>
+        <f t="shared" ref="C233:C234" si="61">C228/ (A228*LOG(A228, 2))</f>
         <v>0.95525420201371603</v>
       </c>
       <c r="D233" s="2">
-        <f t="shared" ref="D233:D234" si="58">D228/ (A228*LOG(A228, 2))</f>
+        <f t="shared" ref="D233:D234" si="62">D228/ (A228*LOG(A228, 2))</f>
         <v>1.1729273749172213</v>
       </c>
       <c r="E233" s="1">
-        <f t="shared" ref="E233:E234" si="59">E228/ (A228*LOG(A228, 2))</f>
+        <f t="shared" ref="E233:E234" si="63">E228/ (A228*LOG(A228, 2))</f>
         <v>1.1492954408500429</v>
       </c>
     </row>
@@ -34619,19 +36247,19 @@
         <v>100000000</v>
       </c>
       <c r="B234" s="2">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.96781624426130519</v>
       </c>
       <c r="C234" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.96136865926301329</v>
       </c>
       <c r="D234" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>1.1890013385084803</v>
       </c>
       <c r="E234" s="1">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>1.1914730566689777</v>
       </c>
     </row>
@@ -34739,19 +36367,19 @@
         <v>10000000</v>
       </c>
       <c r="B248" s="2">
-        <f t="shared" ref="B248:B249" si="60">B243/ (A243*LOG(A243, 2))</f>
+        <f t="shared" ref="B248:B249" si="64">B243/ (A243*LOG(A243, 2))</f>
         <v>2.0849057498787085</v>
       </c>
       <c r="C248" s="2">
-        <f t="shared" ref="C248:C249" si="61">C243/ (A243*LOG(A243, 2))</f>
+        <f t="shared" ref="C248:C249" si="65">C243/ (A243*LOG(A243, 2))</f>
         <v>2.1144252716053678</v>
       </c>
       <c r="D248" s="2">
-        <f t="shared" ref="D248:D249" si="62">D243/ (A243*LOG(A243, 2))</f>
+        <f t="shared" ref="D248:D249" si="66">D243/ (A243*LOG(A243, 2))</f>
         <v>2.0941647401763421</v>
       </c>
       <c r="E248" s="1">
-        <f t="shared" ref="E248:E249" si="63">E243/ (A243*LOG(A243, 2))</f>
+        <f t="shared" ref="E248:E249" si="67">E243/ (A243*LOG(A243, 2))</f>
         <v>2.1107538925765361</v>
       </c>
     </row>
@@ -34760,19 +36388,19 @@
         <v>100000000</v>
       </c>
       <c r="B249" s="2">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>2.0985089090967728</v>
       </c>
       <c r="C249" s="2">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>2.116242268178405</v>
       </c>
       <c r="D249" s="2">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>2.1452802405530811</v>
       </c>
       <c r="E249" s="1">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.1666684507191443</v>
       </c>
     </row>
@@ -34856,19 +36484,19 @@
         <v>10000000</v>
       </c>
       <c r="B267" s="2">
-        <f t="shared" ref="B267:B268" si="64">B262/ (A262*LOG(A262, 2))</f>
+        <f t="shared" ref="B267:B268" si="68">B262/ (A262*LOG(A262, 2))</f>
         <v>6.463027998335486E-3</v>
       </c>
       <c r="C267" s="2">
-        <f t="shared" ref="C267:C268" si="65">C262/ (A262*LOG(A262, 2))</f>
+        <f t="shared" ref="C267:C268" si="69">C262/ (A262*LOG(A262, 2))</f>
         <v>6.3754841751678904E-3</v>
       </c>
       <c r="D267" s="2">
-        <f t="shared" ref="D267:D268" si="66">D262/ (A262*LOG(A262, 2))</f>
+        <f t="shared" ref="D267:D268" si="70">D262/ (A262*LOG(A262, 2))</f>
         <v>6.2602154893996427E-3</v>
       </c>
       <c r="E267" s="1">
-        <f t="shared" ref="E267:E268" si="67">E262/ (A262*LOG(A262, 2))</f>
+        <f t="shared" ref="E267:E268" si="71">E262/ (A262*LOG(A262, 2))</f>
         <v>6.4603961360876812E-3</v>
       </c>
     </row>
@@ -34877,19 +36505,19 @@
         <v>100000000</v>
       </c>
       <c r="B268" s="2">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>6.4025595655528983E-3</v>
       </c>
       <c r="C268" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>6.3997208526937865E-3</v>
       </c>
       <c r="D268" s="2">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>6.2968668052127905E-3</v>
       </c>
       <c r="E268" s="1">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>6.5666032276775225E-3</v>
       </c>
     </row>
@@ -34970,19 +36598,19 @@
         <v>10000000</v>
       </c>
       <c r="B280" s="2">
-        <f t="shared" ref="B280:B281" si="68" xml:space="preserve"> B275/ (A275*LOG(A275, 2))</f>
+        <f t="shared" ref="B280:B281" si="72" xml:space="preserve"> B275/ (A275*LOG(A275, 2))</f>
         <v>0.94652947545195787</v>
       </c>
       <c r="C280" s="2">
-        <f t="shared" ref="C280:C281" si="69" xml:space="preserve"> C275/ (A275*LOG(A275, 2))</f>
+        <f t="shared" ref="C280:C281" si="73" xml:space="preserve"> C275/ (A275*LOG(A275, 2))</f>
         <v>0.96331240516078898</v>
       </c>
       <c r="D280" s="2">
-        <f t="shared" ref="D280:D281" si="70" xml:space="preserve"> D275/ (A275*LOG(A275, 2))</f>
+        <f t="shared" ref="D280:D281" si="74" xml:space="preserve"> D275/ (A275*LOG(A275, 2))</f>
         <v>0.94652947975238644</v>
       </c>
       <c r="E280" s="1">
-        <f t="shared" ref="E280:E281" si="71" xml:space="preserve"> E275/ (A275*LOG(A275, 2))</f>
+        <f t="shared" ref="E280:E281" si="75" xml:space="preserve"> E275/ (A275*LOG(A275, 2))</f>
         <v>0.97802004268036957</v>
       </c>
     </row>
@@ -34991,19 +36619,19 @@
         <v>100000000</v>
       </c>
       <c r="B281" s="2">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0.95310602707592784</v>
       </c>
       <c r="C281" s="2">
-        <f t="shared" si="69"/>
+        <f t="shared" si="73"/>
         <v>0.95582592602976302</v>
       </c>
       <c r="D281" s="2">
-        <f t="shared" si="70"/>
+        <f t="shared" si="74"/>
         <v>0.95310602707592784</v>
       </c>
       <c r="E281" s="1">
-        <f t="shared" si="71"/>
+        <f t="shared" si="75"/>
         <v>0.97677746057896586</v>
       </c>
     </row>
@@ -35084,19 +36712,19 @@
         <v>10000000</v>
       </c>
       <c r="B292" s="2">
-        <f t="shared" ref="B292:B293" si="72">B287/ (A287*LOG(A287, 2))</f>
+        <f t="shared" ref="B292:B293" si="76">B287/ (A287*LOG(A287, 2))</f>
         <v>0.97106040119775872</v>
       </c>
       <c r="C292" s="2">
-        <f t="shared" ref="C292:C293" si="73">C287/ (A287*LOG(A287, 2))</f>
+        <f t="shared" ref="C292:C293" si="77">C287/ (A287*LOG(A287, 2))</f>
         <v>1.0321028422765068</v>
       </c>
       <c r="D292" s="2">
-        <f t="shared" ref="D292:D293" si="74">D287/ (A287*LOG(A287, 2))</f>
+        <f t="shared" ref="D292:D293" si="78">D287/ (A287*LOG(A287, 2))</f>
         <v>0.97106040119775872</v>
       </c>
       <c r="E292" s="1">
-        <f t="shared" ref="E292:E293" si="75">E287/ (A287*LOG(A287, 2))</f>
+        <f t="shared" ref="E292:E293" si="79">E287/ (A287*LOG(A287, 2))</f>
         <v>1.0259607767599768</v>
       </c>
     </row>
@@ -35105,19 +36733,19 @@
         <v>100000000</v>
       </c>
       <c r="B293" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>0.97834748590793874</v>
       </c>
       <c r="C293" s="2">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>1.0159762353659365</v>
       </c>
       <c r="D293" s="2">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>0.97834748590793874</v>
       </c>
       <c r="E293" s="1">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>1.0482312325210248</v>
       </c>
     </row>
@@ -35207,19 +36835,19 @@
         <v>100000000</v>
       </c>
       <c r="B309" s="2">
-        <f t="shared" ref="B309:B310" si="76">B304/ (A304)</f>
+        <f t="shared" ref="B309:B310" si="80">B304/ (A304)</f>
         <v>3.4047109999999998E-2</v>
       </c>
       <c r="C309" s="2">
-        <f t="shared" ref="C309:C310" si="77">C304/ (A304)</f>
+        <f t="shared" ref="C309:C310" si="81">C304/ (A304)</f>
         <v>6.4346799999999999E-3</v>
       </c>
       <c r="D309" s="2">
-        <f t="shared" ref="D309:D310" si="78">D304/ (A304)</f>
+        <f t="shared" ref="D309:D310" si="82">D304/ (A304)</f>
         <v>1.3536090000000001E-2</v>
       </c>
       <c r="E309" s="1">
-        <f t="shared" ref="E309:E310" si="79">E304/ (A304)</f>
+        <f t="shared" ref="E309:E310" si="83">E304/ (A304)</f>
         <v>1.435197E-2</v>
       </c>
     </row>
@@ -35228,19 +36856,19 @@
         <v>1000000000</v>
       </c>
       <c r="B310" s="2">
-        <f t="shared" si="76"/>
+        <f t="shared" si="80"/>
         <v>3.4696666000000001E-2</v>
       </c>
       <c r="C310" s="2">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>6.4368699999999999E-3</v>
       </c>
       <c r="D310" s="2">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>1.5808005999999999E-2</v>
       </c>
       <c r="E310" s="1">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>1.421007E-2</v>
       </c>
     </row>
@@ -35351,19 +36979,19 @@
         <v>100000000</v>
       </c>
       <c r="B325" s="2">
-        <f t="shared" ref="B325:B326" si="80">B320/ (A320)</f>
+        <f t="shared" ref="B325:B326" si="84">B320/ (A320)</f>
         <v>1.1291206600000001</v>
       </c>
       <c r="C325" s="2">
-        <f t="shared" ref="C325:C326" si="81">C320/ (A320)</f>
+        <f t="shared" ref="C325:C326" si="85">C320/ (A320)</f>
         <v>0.99999998000000001</v>
       </c>
       <c r="D325" s="2">
-        <f t="shared" ref="D325:D326" si="82">D320/ (A320)</f>
+        <f t="shared" ref="D325:D326" si="86">D320/ (A320)</f>
         <v>1.5016591500000001</v>
       </c>
       <c r="E325" s="1">
-        <f t="shared" ref="E325:E326" si="83">E320/ (A320)</f>
+        <f t="shared" ref="E325:E326" si="87">E320/ (A320)</f>
         <v>0.99999996999999996</v>
       </c>
     </row>
@@ -35372,19 +37000,19 @@
         <v>1000000000</v>
       </c>
       <c r="B326" s="2">
-        <f t="shared" si="80"/>
+        <f t="shared" si="84"/>
         <v>1.1263233180000001</v>
       </c>
       <c r="C326" s="2">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.99999999799999995</v>
       </c>
       <c r="D326" s="2">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>1.5012655029999999</v>
       </c>
       <c r="E326" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="87"/>
         <v>0.99999999900000003</v>
       </c>
     </row>
@@ -35489,19 +37117,19 @@
         <v>100000000</v>
       </c>
       <c r="B339" s="2">
-        <f t="shared" ref="B339:B340" si="84">B334/ (A334)</f>
+        <f t="shared" ref="B339:B340" si="88">B334/ (A334)</f>
         <v>3.0067932700000002</v>
       </c>
       <c r="C339" s="2">
-        <f t="shared" ref="C339:C340" si="85">C334/ (A334)</f>
+        <f t="shared" ref="C339:C340" si="89">C334/ (A334)</f>
         <v>2.9999999700000002</v>
       </c>
       <c r="D339" s="2">
-        <f t="shared" ref="D339:D340" si="86">D334/ (A334)</f>
+        <f t="shared" ref="D339:D340" si="90">D334/ (A334)</f>
         <v>4.0009259999999998</v>
       </c>
       <c r="E339" s="1">
-        <f t="shared" ref="E339:E340" si="87">E334/ (A334)</f>
+        <f t="shared" ref="E339:E340" si="91">E334/ (A334)</f>
         <v>1.4999999900000001</v>
       </c>
     </row>
@@ -35510,19 +37138,19 @@
         <v>1000000000</v>
       </c>
       <c r="B340" s="2">
-        <f t="shared" si="84"/>
+        <f t="shared" si="88"/>
         <v>3.002293469</v>
       </c>
       <c r="C340" s="2">
-        <f t="shared" si="85"/>
+        <f t="shared" si="89"/>
         <v>2.9999999939999999</v>
       </c>
       <c r="D340" s="2">
-        <f t="shared" si="86"/>
+        <f t="shared" si="90"/>
         <v>4.0236719169999997</v>
       </c>
       <c r="E340" s="1">
-        <f t="shared" si="87"/>
+        <f t="shared" si="91"/>
         <v>1.5</v>
       </c>
     </row>
@@ -35612,11 +37240,11 @@
         <v>100000000</v>
       </c>
       <c r="B359" s="2">
-        <f t="shared" ref="B359:B360" si="88">B354/ (A354*LOG(A354, 2))</f>
+        <f t="shared" ref="B359:B360" si="92">B354/ (A354*LOG(A354, 2))</f>
         <v>8.3264306029290705E-3</v>
       </c>
       <c r="C359" s="2">
-        <f t="shared" ref="C359:C360" si="89">C354/ (A354*LOG(A354, 2))</f>
+        <f t="shared" ref="C359:C360" si="93">C354/ (A354*LOG(A354, 2))</f>
         <v>6.9685275655507273E-3</v>
       </c>
       <c r="D359" s="2">
@@ -35624,7 +37252,7 @@
         <v>1.079903266275135E-2</v>
       </c>
       <c r="E359" s="1">
-        <f t="shared" ref="E359:E360" si="90">E354/ (A354*LOG(A354, 2))</f>
+        <f t="shared" ref="E359:E360" si="94">E354/ (A354*LOG(A354, 2))</f>
         <v>9.1996753472884021E-3</v>
       </c>
     </row>
@@ -35633,19 +37261,19 @@
         <v>1000000000</v>
       </c>
       <c r="B360" s="2">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>8.4526406814075371E-3</v>
       </c>
       <c r="C360" s="2">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>7.0019156887359182E-3</v>
       </c>
       <c r="D360" s="2">
-        <f t="shared" ref="D360" si="91">D355/ (A355*LOG(A355, 2))</f>
+        <f t="shared" ref="D360" si="95">D355/ (A355*LOG(A355, 2))</f>
         <v>1.110553976539533E-2</v>
       </c>
       <c r="E360" s="1">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>9.6227512316911096E-3</v>
       </c>
     </row>
@@ -35750,19 +37378,19 @@
         <v>100000000</v>
       </c>
       <c r="B373" s="2">
-        <f t="shared" ref="B373:B374" si="92">B368/ (A368*LOG(A368, 2))</f>
+        <f t="shared" ref="B373:B374" si="96">B368/ (A368*LOG(A368, 2))</f>
         <v>1.1895211819399674</v>
       </c>
       <c r="C373" s="2">
-        <f t="shared" ref="C373:C374" si="93">C368/ (A368*LOG(A368, 2))</f>
+        <f t="shared" ref="C373:C374" si="97">C368/ (A368*LOG(A368, 2))</f>
         <v>1.1348620205844124</v>
       </c>
       <c r="D373" s="2">
-        <f t="shared" ref="D373:D374" si="94">D368/ (A368*LOG(A368, 2))</f>
+        <f t="shared" ref="D373:D374" si="98">D368/ (A368*LOG(A368, 2))</f>
         <v>1.1646660571023542</v>
       </c>
       <c r="E373" s="1">
-        <f t="shared" ref="E373:E374" si="95">E368/ (A368*LOG(A368, 2))</f>
+        <f t="shared" ref="E373:E374" si="99">E368/ (A368*LOG(A368, 2))</f>
         <v>1.5177653623839071</v>
       </c>
     </row>
@@ -35771,19 +37399,19 @@
         <v>1000000000</v>
       </c>
       <c r="B374" s="2">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>1.2303861803970835</v>
       </c>
       <c r="C374" s="2">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>1.1580056035758324</v>
       </c>
       <c r="D374" s="2">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>1.1721572097754291</v>
       </c>
       <c r="E374" s="1">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>1.535540542944053</v>
       </c>
     </row>
@@ -35891,19 +37519,19 @@
         <v>100000000</v>
       </c>
       <c r="B388" s="2">
-        <f t="shared" ref="B388:B389" si="96">B383/ (A383*LOG(A383, 2))</f>
+        <f t="shared" ref="B388:B389" si="100">B383/ (A383*LOG(A383, 2))</f>
         <v>2.1457446654912289</v>
       </c>
       <c r="C388" s="2">
-        <f t="shared" ref="C388:C389" si="97">C383/ (A383*LOG(A383, 2))</f>
+        <f t="shared" ref="C388:C389" si="101">C383/ (A383*LOG(A383, 2))</f>
         <v>1.9610036544065781</v>
       </c>
       <c r="D388" s="2">
-        <f t="shared" ref="D388:D389" si="98">D383/ (A383*LOG(A383, 2))</f>
+        <f t="shared" ref="D388:D389" si="102">D383/ (A383*LOG(A383, 2))</f>
         <v>3.466242459528742</v>
       </c>
       <c r="E388" s="1">
-        <f t="shared" ref="E388:E389" si="99">E383/ (A383*LOG(A383, 2))</f>
+        <f t="shared" ref="E388:E389" si="103">E383/ (A383*LOG(A383, 2))</f>
         <v>3.7255515984218306</v>
       </c>
     </row>
@@ -35912,19 +37540,19 @@
         <v>1000000000</v>
       </c>
       <c r="B389" s="2">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>2.1472442034760451</v>
       </c>
       <c r="C389" s="2">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>1.9927756519439235</v>
       </c>
       <c r="D389" s="2">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>3.6523597798539122</v>
       </c>
       <c r="E389" s="1">
-        <f t="shared" si="99"/>
+        <f t="shared" si="103"/>
         <v>3.7594986531061276</v>
       </c>
     </row>
@@ -36010,15 +37638,15 @@
         <v>10000000</v>
       </c>
       <c r="B406" s="2">
-        <f t="shared" ref="B406:B407" si="100">B401/ (A401*LOG(A401, 2))</f>
+        <f t="shared" ref="B406:B407" si="104">B401/ (A401*LOG(A401, 2))</f>
         <v>1.0092065008063044E-2</v>
       </c>
       <c r="C406" s="2">
-        <f t="shared" ref="C406:C407" si="101">C401/ (A401*LOG(A401, 2))</f>
+        <f t="shared" ref="C406:C407" si="105">C401/ (A401*LOG(A401, 2))</f>
         <v>8.2734481948297262E-3</v>
       </c>
       <c r="D406" s="2">
-        <f t="shared" ref="D406:D407" si="102">D401/ (A401*LOG(A401, 2))</f>
+        <f t="shared" ref="D406:D407" si="106">D401/ (A401*LOG(A401, 2))</f>
         <v>1.1267053887995714E-2</v>
       </c>
     </row>
@@ -36027,15 +37655,15 @@
         <v>100000000</v>
       </c>
       <c r="B407" s="2">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>1.0207057176278133E-2</v>
       </c>
       <c r="C407" s="2">
-        <f t="shared" si="101"/>
+        <f t="shared" si="105"/>
         <v>8.4549640141901826E-3</v>
       </c>
       <c r="D407" s="2">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>1.5788662412868509E-2</v>
       </c>
     </row>
@@ -36103,15 +37731,15 @@
         <v>10000000</v>
       </c>
       <c r="B420" s="2">
-        <f t="shared" ref="B420:B421" si="103">B415/ (A415*LOG(A415, 2))</f>
+        <f t="shared" ref="B420:B421" si="107">B415/ (A415*LOG(A415, 2))</f>
         <v>1.1103958760636357</v>
       </c>
       <c r="C420" s="2">
-        <f t="shared" ref="C420:C421" si="104">C415/ (A415*LOG(A415, 2))</f>
+        <f t="shared" ref="C420:C421" si="108">C415/ (A415*LOG(A415, 2))</f>
         <v>1.1755109046490082</v>
       </c>
       <c r="D420" s="2">
-        <f t="shared" ref="D420:D421" si="105">D415/ (A415*LOG(A415, 2))</f>
+        <f t="shared" ref="D420:D421" si="109">D415/ (A415*LOG(A415, 2))</f>
         <v>1.0207752125525265</v>
       </c>
     </row>
@@ -36120,15 +37748,15 @@
         <v>100000000</v>
       </c>
       <c r="B421" s="2">
-        <f t="shared" si="103"/>
+        <f t="shared" si="107"/>
         <v>1.2083626960282254</v>
       </c>
       <c r="C421" s="2">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>1.1910224768529054</v>
       </c>
       <c r="D421" s="2">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>1.0185743119959765</v>
       </c>
     </row>
@@ -36196,15 +37824,15 @@
         <v>10000000</v>
       </c>
       <c r="B433" s="2">
-        <f t="shared" ref="B433:B434" si="106">B428/ (A428*LOG(A428, 2))</f>
+        <f t="shared" ref="B433:B434" si="110">B428/ (A428*LOG(A428, 2))</f>
         <v>1.9980186451487967</v>
       </c>
       <c r="C433" s="2">
-        <f t="shared" ref="C433:C434" si="107">C428/ (A428*LOG(A428, 2))</f>
+        <f t="shared" ref="C433:C434" si="111">C428/ (A428*LOG(A428, 2))</f>
         <v>2.0947274082425236</v>
       </c>
       <c r="D433" s="2">
-        <f t="shared" ref="D433:D434" si="108">D428/ (A428*LOG(A428, 2))</f>
+        <f t="shared" ref="D433:D434" si="112">D428/ (A428*LOG(A428, 2))</f>
         <v>1.9896927446274366</v>
       </c>
     </row>
@@ -36213,15 +37841,15 @@
         <v>100000000</v>
       </c>
       <c r="B434" s="2">
-        <f t="shared" si="106"/>
+        <f t="shared" si="110"/>
         <v>2.0825999626233869</v>
       </c>
       <c r="C434" s="2">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>2.1457233059078868</v>
       </c>
       <c r="D434" s="2">
-        <f t="shared" si="108"/>
+        <f t="shared" si="112"/>
         <v>1.9917439717262588</v>
       </c>
     </row>

</xml_diff>